<commit_message>
more cleaning data sheets, division of models more clear for question 1, subdividing wasting periods and comparing of pre-present and post-present. Added dates
</commit_message>
<xml_diff>
--- a/historic_raw_data/data from isa/Spiny sea star sizes.xlsx
+++ b/historic_raw_data/data from isa/Spiny sea star sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicole/Desktop/honours_project/pink_sea_star_indian_arm/historic_raw_data/data from isa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E05D5CF-3B96-F149-8AF2-CBD9EFAA13D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B895BE-2B0C-B840-BA8C-86DC97A073B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A3D9EDB8-C9F0-4048-A7AA-C6D7C228C698}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{A3D9EDB8-C9F0-4048-A7AA-C6D7C228C698}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="192">
   <si>
     <t>Size distribution - Moody Inlet</t>
   </si>
@@ -602,6 +602,24 @@
   </si>
   <si>
     <t>White Rock (actualy Grey Rock)</t>
+  </si>
+  <si>
+    <t>Time: 42 minutes</t>
+  </si>
+  <si>
+    <t>time: 30 minutes</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>42 minutes</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>37 minutes</t>
   </si>
 </sst>
 </file>
@@ -982,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F1ABEE-9A9C-C243-811B-BFEE9BEB4494}">
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="132" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A3" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2952,7 +2970,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:H1"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3537,7 +3555,7 @@
   <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3568,6 +3586,9 @@
       </c>
       <c r="D3" t="s">
         <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
@@ -3937,8 +3958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF73E783-9AF6-BA44-A2FF-8EACC436F975}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView zoomScale="134" workbookViewId="0">
-      <selection activeCell="C38" sqref="C4:C38"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4290,15 +4311,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2CB9EA-4359-D447-8162-9B636C05F291}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B43"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -4309,7 +4330,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -4320,7 +4341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4330,8 +4351,11 @@
       <c r="C4">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J4" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>17.2</v>
       </c>
@@ -4339,7 +4363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>17.5</v>
       </c>
@@ -4350,7 +4374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>19</v>
       </c>
@@ -4358,7 +4382,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B8">
         <v>15</v>
       </c>
@@ -4366,7 +4390,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B9">
         <v>19</v>
       </c>
@@ -4374,7 +4398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B10">
         <v>15.2</v>
       </c>
@@ -4382,7 +4406,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B11">
         <v>20.5</v>
       </c>
@@ -4399,7 +4423,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B12">
         <v>20.2</v>
       </c>
@@ -4417,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B13">
         <v>13</v>
       </c>
@@ -4435,7 +4459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B14">
         <v>15</v>
       </c>
@@ -4453,7 +4477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B15">
         <v>19</v>
       </c>
@@ -4471,7 +4495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B16">
         <v>17.5</v>
       </c>
@@ -4808,7 +4832,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="164" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4836,6 +4860,12 @@
       </c>
       <c r="E3" t="s">
         <v>9</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -5122,8 +5152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EACA228-D9EE-CB4D-A792-EA7D45D2C56B}">
   <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView zoomScale="241" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D83"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6228,8 +6258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F980C4-88A1-FE4F-8DCC-B5CA81468457}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D75"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6289,6 +6319,12 @@
       </c>
       <c r="D6">
         <v>12.3</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>